<commit_message>
fix utibill form no border and spa pos
</commit_message>
<xml_diff>
--- a/assets/water/invoice_cash_auto.xlsx
+++ b/assets/water/invoice_cash_auto.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24709"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="20020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="box" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>number</t>
   </si>
@@ -31,6 +31,12 @@
   </si>
   <si>
     <t>INV00001</t>
+  </si>
+  <si>
+    <t>issued_date</t>
+  </si>
+  <si>
+    <t>2018-01-01</t>
   </si>
 </sst>
 </file>
@@ -71,7 +77,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -96,10 +102,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -377,7 +384,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -385,32 +392,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22.1640625" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>100000</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>